<commit_message>
Working on Database modelling assessment
</commit_message>
<xml_diff>
--- a/Off The Job Calculator - Joshua Morton.xlsx
+++ b/Off The Job Calculator - Joshua Morton.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoshMorton\Documents\_Degree\DegreePub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945CF56F-D14D-478C-97EB-3982ACB7215A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1429A4F-9A33-437D-BB26-ABF6747525CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="18720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10822" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10846" uniqueCount="440">
   <si>
     <t>How to complete this calculator</t>
   </si>
@@ -1483,6 +1483,15 @@
   <si>
     <t>Professional Practice and Portfolio Development 1</t>
   </si>
+  <si>
+    <t>25/07/2023</t>
+  </si>
+  <si>
+    <t>26/07/2023</t>
+  </si>
+  <si>
+    <t>01/08/2023</t>
+  </si>
 </sst>
 </file>
 
@@ -2285,45 +2294,11 @@
     <xf numFmtId="49" fontId="15" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2350,6 +2325,40 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4069,25 +4078,25 @@
   <sheetData>
     <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
-      <c r="N7" s="99"/>
-      <c r="O7" s="99"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="99"/>
-      <c r="R7" s="100"/>
+      <c r="B7" s="107" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="108"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="108"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="108"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="108"/>
+      <c r="R7" s="109"/>
     </row>
     <row r="8" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
@@ -4109,135 +4118,135 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="93" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="94"/>
-      <c r="O9" s="94"/>
-      <c r="P9" s="94"/>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="94"/>
+      <c r="B9" s="104" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="105"/>
+      <c r="M9" s="105"/>
+      <c r="N9" s="105"/>
+      <c r="O9" s="105"/>
+      <c r="P9" s="105"/>
+      <c r="Q9" s="105"/>
+      <c r="R9" s="105"/>
     </row>
     <row r="10" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="87" t="s">
+      <c r="B10" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
-      <c r="L10" s="88"/>
-      <c r="M10" s="88"/>
-      <c r="N10" s="88"/>
-      <c r="O10" s="88"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="89"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="102"/>
+      <c r="I10" s="102"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="102"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
+      <c r="O10" s="102"/>
+      <c r="P10" s="102"/>
+      <c r="Q10" s="102"/>
+      <c r="R10" s="103"/>
     </row>
     <row r="11" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="88"/>
-      <c r="L11" s="88"/>
-      <c r="M11" s="88"/>
-      <c r="N11" s="88"/>
-      <c r="O11" s="88"/>
-      <c r="P11" s="88"/>
-      <c r="Q11" s="88"/>
-      <c r="R11" s="89"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="102"/>
+      <c r="N11" s="102"/>
+      <c r="O11" s="102"/>
+      <c r="P11" s="102"/>
+      <c r="Q11" s="102"/>
+      <c r="R11" s="103"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="95" t="s">
+      <c r="B12" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="96"/>
-      <c r="F12" s="96"/>
-      <c r="G12" s="96"/>
-      <c r="H12" s="96"/>
-      <c r="I12" s="96"/>
-      <c r="J12" s="96"/>
-      <c r="K12" s="96"/>
-      <c r="L12" s="96"/>
-      <c r="M12" s="96"/>
-      <c r="N12" s="96"/>
-      <c r="O12" s="96"/>
-      <c r="P12" s="96"/>
-      <c r="Q12" s="96"/>
-      <c r="R12" s="97"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="88"/>
     </row>
     <row r="13" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="102"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="102"/>
-      <c r="L13" s="102"/>
-      <c r="M13" s="102"/>
-      <c r="N13" s="102"/>
-      <c r="O13" s="102"/>
-      <c r="P13" s="102"/>
-      <c r="Q13" s="102"/>
-      <c r="R13" s="103"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="111"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="111"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="111"/>
+      <c r="R13" s="112"/>
     </row>
     <row r="14" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="91"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="91"/>
-      <c r="K14" s="91"/>
-      <c r="L14" s="91"/>
-      <c r="M14" s="91"/>
-      <c r="N14" s="91"/>
-      <c r="O14" s="91"/>
-      <c r="P14" s="91"/>
-      <c r="Q14" s="91"/>
-      <c r="R14" s="92"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="90"/>
+      <c r="M14" s="90"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="90"/>
+      <c r="P14" s="90"/>
+      <c r="Q14" s="90"/>
+      <c r="R14" s="91"/>
     </row>
     <row r="15" spans="1:18" ht="5.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
@@ -4259,91 +4268,91 @@
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B16" s="104" t="s">
+      <c r="B16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="105"/>
-      <c r="K16" s="105"/>
-      <c r="L16" s="105"/>
-      <c r="M16" s="105"/>
-      <c r="N16" s="105"/>
-      <c r="O16" s="105"/>
-      <c r="P16" s="105"/>
-      <c r="Q16" s="105"/>
-      <c r="R16" s="105"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="93"/>
+      <c r="M16" s="93"/>
+      <c r="N16" s="93"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="93"/>
     </row>
     <row r="17" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-      <c r="B17" s="96" t="s">
+      <c r="B17" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="97"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="87"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="87"/>
+      <c r="O17" s="87"/>
+      <c r="P17" s="87"/>
+      <c r="Q17" s="87"/>
+      <c r="R17" s="88"/>
     </row>
     <row r="18" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="96"/>
-      <c r="J18" s="96"/>
-      <c r="K18" s="96"/>
-      <c r="L18" s="96"/>
-      <c r="M18" s="96"/>
-      <c r="N18" s="96"/>
-      <c r="O18" s="96"/>
-      <c r="P18" s="96"/>
-      <c r="Q18" s="96"/>
-      <c r="R18" s="97"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="87"/>
+      <c r="M18" s="87"/>
+      <c r="N18" s="87"/>
+      <c r="O18" s="87"/>
+      <c r="P18" s="87"/>
+      <c r="Q18" s="87"/>
+      <c r="R18" s="88"/>
     </row>
     <row r="19" spans="1:18" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="108"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="108"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="108"/>
-      <c r="K19" s="108"/>
-      <c r="L19" s="108"/>
-      <c r="M19" s="108"/>
-      <c r="N19" s="108"/>
-      <c r="O19" s="108"/>
-      <c r="P19" s="108"/>
-      <c r="Q19" s="108"/>
-      <c r="R19" s="109"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="96"/>
+      <c r="I19" s="96"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="96"/>
+      <c r="L19" s="96"/>
+      <c r="M19" s="96"/>
+      <c r="N19" s="96"/>
+      <c r="O19" s="96"/>
+      <c r="P19" s="96"/>
+      <c r="Q19" s="96"/>
+      <c r="R19" s="97"/>
     </row>
     <row r="20" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
@@ -4365,112 +4374,112 @@
       <c r="R20" s="5"/>
     </row>
     <row r="21" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B21" s="106" t="s">
+      <c r="B21" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="107"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="107"/>
-      <c r="H21" s="107"/>
-      <c r="I21" s="107"/>
-      <c r="J21" s="107"/>
-      <c r="K21" s="107"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="107"/>
-      <c r="N21" s="107"/>
-      <c r="O21" s="107"/>
-      <c r="P21" s="107"/>
-      <c r="Q21" s="107"/>
-      <c r="R21" s="107"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="95"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="95"/>
+      <c r="K21" s="95"/>
+      <c r="L21" s="95"/>
+      <c r="M21" s="95"/>
+      <c r="N21" s="95"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="95"/>
+      <c r="R21" s="95"/>
     </row>
     <row r="22" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="96"/>
-      <c r="I22" s="96"/>
-      <c r="J22" s="96"/>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="96"/>
-      <c r="O22" s="96"/>
-      <c r="P22" s="96"/>
-      <c r="Q22" s="96"/>
-      <c r="R22" s="97"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="87"/>
+      <c r="M22" s="87"/>
+      <c r="N22" s="87"/>
+      <c r="O22" s="87"/>
+      <c r="P22" s="87"/>
+      <c r="Q22" s="87"/>
+      <c r="R22" s="88"/>
     </row>
     <row r="23" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="B23" s="96" t="s">
+      <c r="B23" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="96"/>
-      <c r="I23" s="96"/>
-      <c r="J23" s="96"/>
-      <c r="K23" s="96"/>
-      <c r="L23" s="96"/>
-      <c r="M23" s="96"/>
-      <c r="N23" s="96"/>
-      <c r="O23" s="96"/>
-      <c r="P23" s="96"/>
-      <c r="Q23" s="96"/>
-      <c r="R23" s="97"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="87"/>
+      <c r="J23" s="87"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="87"/>
+      <c r="M23" s="87"/>
+      <c r="N23" s="87"/>
+      <c r="O23" s="87"/>
+      <c r="P23" s="87"/>
+      <c r="Q23" s="87"/>
+      <c r="R23" s="88"/>
     </row>
     <row r="24" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="110" t="s">
+      <c r="B24" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="111"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="111"/>
-      <c r="H24" s="111"/>
-      <c r="I24" s="111"/>
-      <c r="J24" s="111"/>
-      <c r="K24" s="111"/>
-      <c r="L24" s="111"/>
-      <c r="M24" s="111"/>
-      <c r="N24" s="111"/>
-      <c r="O24" s="111"/>
-      <c r="P24" s="111"/>
-      <c r="Q24" s="111"/>
-      <c r="R24" s="112"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="99"/>
+      <c r="J24" s="99"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="99"/>
+      <c r="M24" s="99"/>
+      <c r="N24" s="99"/>
+      <c r="O24" s="99"/>
+      <c r="P24" s="99"/>
+      <c r="Q24" s="99"/>
+      <c r="R24" s="100"/>
     </row>
     <row r="25" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B25" s="90" t="s">
+      <c r="B25" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="91"/>
-      <c r="I25" s="91"/>
-      <c r="J25" s="91"/>
-      <c r="K25" s="91"/>
-      <c r="L25" s="91"/>
-      <c r="M25" s="91"/>
-      <c r="N25" s="91"/>
-      <c r="O25" s="91"/>
-      <c r="P25" s="91"/>
-      <c r="Q25" s="91"/>
-      <c r="R25" s="92"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="90"/>
+      <c r="H25" s="90"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="90"/>
+      <c r="N25" s="90"/>
+      <c r="O25" s="90"/>
+      <c r="P25" s="90"/>
+      <c r="Q25" s="90"/>
+      <c r="R25" s="91"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="R26" s="2"/>
@@ -4478,6 +4487,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="C1AqtvqKb8C414s7lEoNpdJ58hWR+bz87IU733aDeZMTPECU7crf3JYNQw8QcQksZnMw+dDwa8mNa2TsA5r9Aw==" saltValue="4/m+8HEyihP2IsZnh8JafA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="16">
+    <mergeCell ref="B10:R10"/>
+    <mergeCell ref="B14:R14"/>
+    <mergeCell ref="B9:R9"/>
+    <mergeCell ref="B12:R12"/>
+    <mergeCell ref="B7:R7"/>
+    <mergeCell ref="B11:R11"/>
+    <mergeCell ref="B13:R13"/>
     <mergeCell ref="B22:R22"/>
     <mergeCell ref="B23:R23"/>
     <mergeCell ref="B25:R25"/>
@@ -4487,13 +4503,6 @@
     <mergeCell ref="B18:R18"/>
     <mergeCell ref="B19:R19"/>
     <mergeCell ref="B24:R24"/>
-    <mergeCell ref="B10:R10"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B9:R9"/>
-    <mergeCell ref="B12:R12"/>
-    <mergeCell ref="B7:R7"/>
-    <mergeCell ref="B11:R11"/>
-    <mergeCell ref="B13:R13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -10383,7 +10392,7 @@
   <dimension ref="B1:R202"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10480,7 +10489,7 @@
       </c>
       <c r="J4" s="41">
         <f>I202</f>
-        <v>128.50000000029104</v>
+        <v>143.00000000040745</v>
       </c>
       <c r="L4" s="133"/>
       <c r="R4" t="s">
@@ -10499,7 +10508,7 @@
       </c>
       <c r="J5" s="41">
         <f>J3-J4</f>
-        <v>1414.499999999709</v>
+        <v>1399.9999999995925</v>
       </c>
       <c r="L5" s="133"/>
       <c r="M5" s="32"/>
@@ -11351,67 +11360,115 @@
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="82" t="str">
+      <c r="B37" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="E37" s="82">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="36" t="str">
+        <v>210.00000000349246</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I37" s="36">
         <f t="shared" si="1"/>
-        <v/>
+        <v>3.5000000000582077</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="82" t="str">
+      <c r="B38" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="E38" s="82">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="36" t="str">
+        <v>210.00000000349246</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I38" s="36">
         <f t="shared" si="1"/>
-        <v/>
+        <v>3.5000000000582077</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="82" t="str">
+      <c r="B39" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="E39" s="82">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="36" t="str">
+        <v>210.00000000349246</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I39" s="36">
         <f t="shared" si="1"/>
-        <v/>
+        <v>3.5000000000582077</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="82" t="str">
+      <c r="B40" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="E40" s="82">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="36" t="str">
+        <v>239.99999999650754</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I40" s="36">
         <f t="shared" si="1"/>
-        <v/>
+        <v>3.9999999999417923</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
@@ -14002,7 +14059,7 @@
       <c r="H202" s="35"/>
       <c r="I202" s="83">
         <f>SUM($I$8:I201)</f>
-        <v>128.50000000029104</v>
+        <v>143.00000000040745</v>
       </c>
     </row>
   </sheetData>
@@ -77674,9 +77731,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -77909,19 +77969,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E15B46B-DB71-477E-9F64-462B1A7F47C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5ECEC2-D611-47E4-BF40-446047C7D564}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -77946,9 +78002,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5ECEC2-D611-47E4-BF40-446047C7D564}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E15B46B-DB71-477E-9F64-462B1A7F47C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
OTJC Calc & DCNS
</commit_message>
<xml_diff>
--- a/Off The Job Calculator - Joshua Morton.xlsx
+++ b/Off The Job Calculator - Joshua Morton.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoshMorton\Documents\_Degree\DegreePub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE18C1F-E126-4495-BF32-FA036173A64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4822B6-35F4-4D2A-B97C-09085E5838FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1650" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="4" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11188" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11206" uniqueCount="488">
   <si>
     <t>How to complete this calculator</t>
   </si>
@@ -1630,6 +1630,12 @@
   <si>
     <t>24/01/2024</t>
   </si>
+  <si>
+    <t>31/01/2024</t>
+  </si>
+  <si>
+    <t>04/02/2024</t>
+  </si>
 </sst>
 </file>
 
@@ -2432,11 +2438,45 @@
     <xf numFmtId="49" fontId="15" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2463,40 +2503,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4216,25 +4222,25 @@
   <sheetData>
     <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:18" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
-      <c r="J7" s="108"/>
-      <c r="K7" s="108"/>
-      <c r="L7" s="108"/>
-      <c r="M7" s="108"/>
-      <c r="N7" s="108"/>
-      <c r="O7" s="108"/>
-      <c r="P7" s="108"/>
-      <c r="Q7" s="108"/>
-      <c r="R7" s="109"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="99"/>
+      <c r="N7" s="99"/>
+      <c r="O7" s="99"/>
+      <c r="P7" s="99"/>
+      <c r="Q7" s="99"/>
+      <c r="R7" s="100"/>
     </row>
     <row r="8" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
@@ -4256,135 +4262,135 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B9" s="104" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="105"/>
-      <c r="H9" s="105"/>
-      <c r="I9" s="105"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="105"/>
-      <c r="L9" s="105"/>
-      <c r="M9" s="105"/>
-      <c r="N9" s="105"/>
-      <c r="O9" s="105"/>
-      <c r="P9" s="105"/>
-      <c r="Q9" s="105"/>
-      <c r="R9" s="105"/>
+      <c r="B9" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="94"/>
+      <c r="K9" s="94"/>
+      <c r="L9" s="94"/>
+      <c r="M9" s="94"/>
+      <c r="N9" s="94"/>
+      <c r="O9" s="94"/>
+      <c r="P9" s="94"/>
+      <c r="Q9" s="94"/>
+      <c r="R9" s="94"/>
     </row>
     <row r="10" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
-      <c r="B10" s="101" t="s">
+      <c r="B10" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="102"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="102"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102"/>
-      <c r="K10" s="102"/>
-      <c r="L10" s="102"/>
-      <c r="M10" s="102"/>
-      <c r="N10" s="102"/>
-      <c r="O10" s="102"/>
-      <c r="P10" s="102"/>
-      <c r="Q10" s="102"/>
-      <c r="R10" s="103"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="88"/>
+      <c r="L10" s="88"/>
+      <c r="M10" s="88"/>
+      <c r="N10" s="88"/>
+      <c r="O10" s="88"/>
+      <c r="P10" s="88"/>
+      <c r="Q10" s="88"/>
+      <c r="R10" s="89"/>
     </row>
     <row r="11" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="102"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="102"/>
-      <c r="M11" s="102"/>
-      <c r="N11" s="102"/>
-      <c r="O11" s="102"/>
-      <c r="P11" s="102"/>
-      <c r="Q11" s="102"/>
-      <c r="R11" s="103"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="88"/>
+      <c r="M11" s="88"/>
+      <c r="N11" s="88"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="88"/>
+      <c r="Q11" s="88"/>
+      <c r="R11" s="89"/>
     </row>
     <row r="12" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
-      <c r="B12" s="106" t="s">
+      <c r="B12" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="87"/>
-      <c r="M12" s="87"/>
-      <c r="N12" s="87"/>
-      <c r="O12" s="87"/>
-      <c r="P12" s="87"/>
-      <c r="Q12" s="87"/>
-      <c r="R12" s="88"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="96"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="96"/>
+      <c r="M12" s="96"/>
+      <c r="N12" s="96"/>
+      <c r="O12" s="96"/>
+      <c r="P12" s="96"/>
+      <c r="Q12" s="96"/>
+      <c r="R12" s="97"/>
     </row>
     <row r="13" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
-      <c r="B13" s="110" t="s">
+      <c r="B13" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
-      <c r="L13" s="111"/>
-      <c r="M13" s="111"/>
-      <c r="N13" s="111"/>
-      <c r="O13" s="111"/>
-      <c r="P13" s="111"/>
-      <c r="Q13" s="111"/>
-      <c r="R13" s="112"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
+      <c r="O13" s="102"/>
+      <c r="P13" s="102"/>
+      <c r="Q13" s="102"/>
+      <c r="R13" s="103"/>
     </row>
     <row r="14" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
-      <c r="B14" s="89" t="s">
+      <c r="B14" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
-      <c r="K14" s="90"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="90"/>
-      <c r="O14" s="90"/>
-      <c r="P14" s="90"/>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="91"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="91"/>
+      <c r="K14" s="91"/>
+      <c r="L14" s="91"/>
+      <c r="M14" s="91"/>
+      <c r="N14" s="91"/>
+      <c r="O14" s="91"/>
+      <c r="P14" s="91"/>
+      <c r="Q14" s="91"/>
+      <c r="R14" s="92"/>
     </row>
     <row r="15" spans="1:18" ht="5.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
@@ -4406,91 +4412,91 @@
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="93"/>
-      <c r="K16" s="93"/>
-      <c r="L16" s="93"/>
-      <c r="M16" s="93"/>
-      <c r="N16" s="93"/>
-      <c r="O16" s="93"/>
-      <c r="P16" s="93"/>
-      <c r="Q16" s="93"/>
-      <c r="R16" s="93"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="105"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="105"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="105"/>
+      <c r="N16" s="105"/>
+      <c r="O16" s="105"/>
+      <c r="P16" s="105"/>
+      <c r="Q16" s="105"/>
+      <c r="R16" s="105"/>
     </row>
     <row r="17" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A17" s="2"/>
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="87"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="87"/>
-      <c r="K17" s="87"/>
-      <c r="L17" s="87"/>
-      <c r="M17" s="87"/>
-      <c r="N17" s="87"/>
-      <c r="O17" s="87"/>
-      <c r="P17" s="87"/>
-      <c r="Q17" s="87"/>
-      <c r="R17" s="88"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="96"/>
+      <c r="M17" s="96"/>
+      <c r="N17" s="96"/>
+      <c r="O17" s="96"/>
+      <c r="P17" s="96"/>
+      <c r="Q17" s="96"/>
+      <c r="R17" s="97"/>
     </row>
     <row r="18" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
-      <c r="B18" s="87" t="s">
+      <c r="B18" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="87"/>
-      <c r="K18" s="87"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87"/>
-      <c r="O18" s="87"/>
-      <c r="P18" s="87"/>
-      <c r="Q18" s="87"/>
-      <c r="R18" s="88"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="96"/>
+      <c r="J18" s="96"/>
+      <c r="K18" s="96"/>
+      <c r="L18" s="96"/>
+      <c r="M18" s="96"/>
+      <c r="N18" s="96"/>
+      <c r="O18" s="96"/>
+      <c r="P18" s="96"/>
+      <c r="Q18" s="96"/>
+      <c r="R18" s="97"/>
     </row>
     <row r="19" spans="1:18" ht="32.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="96"/>
-      <c r="I19" s="96"/>
-      <c r="J19" s="96"/>
-      <c r="K19" s="96"/>
-      <c r="L19" s="96"/>
-      <c r="M19" s="96"/>
-      <c r="N19" s="96"/>
-      <c r="O19" s="96"/>
-      <c r="P19" s="96"/>
-      <c r="Q19" s="96"/>
-      <c r="R19" s="97"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="108"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="108"/>
+      <c r="J19" s="108"/>
+      <c r="K19" s="108"/>
+      <c r="L19" s="108"/>
+      <c r="M19" s="108"/>
+      <c r="N19" s="108"/>
+      <c r="O19" s="108"/>
+      <c r="P19" s="108"/>
+      <c r="Q19" s="108"/>
+      <c r="R19" s="109"/>
     </row>
     <row r="20" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="3"/>
@@ -4512,112 +4518,112 @@
       <c r="R20" s="5"/>
     </row>
     <row r="21" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="95"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="95"/>
-      <c r="G21" s="95"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="95"/>
-      <c r="J21" s="95"/>
-      <c r="K21" s="95"/>
-      <c r="L21" s="95"/>
-      <c r="M21" s="95"/>
-      <c r="N21" s="95"/>
-      <c r="O21" s="95"/>
-      <c r="P21" s="95"/>
-      <c r="Q21" s="95"/>
-      <c r="R21" s="95"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="107"/>
+      <c r="E21" s="107"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="107"/>
+      <c r="I21" s="107"/>
+      <c r="J21" s="107"/>
+      <c r="K21" s="107"/>
+      <c r="L21" s="107"/>
+      <c r="M21" s="107"/>
+      <c r="N21" s="107"/>
+      <c r="O21" s="107"/>
+      <c r="P21" s="107"/>
+      <c r="Q21" s="107"/>
+      <c r="R21" s="107"/>
     </row>
     <row r="22" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A22" s="2"/>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="87"/>
-      <c r="J22" s="87"/>
-      <c r="K22" s="87"/>
-      <c r="L22" s="87"/>
-      <c r="M22" s="87"/>
-      <c r="N22" s="87"/>
-      <c r="O22" s="87"/>
-      <c r="P22" s="87"/>
-      <c r="Q22" s="87"/>
-      <c r="R22" s="88"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="96"/>
+      <c r="J22" s="96"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="96"/>
+      <c r="O22" s="96"/>
+      <c r="P22" s="96"/>
+      <c r="Q22" s="96"/>
+      <c r="R22" s="97"/>
     </row>
     <row r="23" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="87"/>
-      <c r="K23" s="87"/>
-      <c r="L23" s="87"/>
-      <c r="M23" s="87"/>
-      <c r="N23" s="87"/>
-      <c r="O23" s="87"/>
-      <c r="P23" s="87"/>
-      <c r="Q23" s="87"/>
-      <c r="R23" s="88"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="96"/>
+      <c r="P23" s="96"/>
+      <c r="Q23" s="96"/>
+      <c r="R23" s="97"/>
     </row>
     <row r="24" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A24" s="2"/>
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="99"/>
-      <c r="D24" s="99"/>
-      <c r="E24" s="99"/>
-      <c r="F24" s="99"/>
-      <c r="G24" s="99"/>
-      <c r="H24" s="99"/>
-      <c r="I24" s="99"/>
-      <c r="J24" s="99"/>
-      <c r="K24" s="99"/>
-      <c r="L24" s="99"/>
-      <c r="M24" s="99"/>
-      <c r="N24" s="99"/>
-      <c r="O24" s="99"/>
-      <c r="P24" s="99"/>
-      <c r="Q24" s="99"/>
-      <c r="R24" s="100"/>
+      <c r="C24" s="111"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="111"/>
+      <c r="G24" s="111"/>
+      <c r="H24" s="111"/>
+      <c r="I24" s="111"/>
+      <c r="J24" s="111"/>
+      <c r="K24" s="111"/>
+      <c r="L24" s="111"/>
+      <c r="M24" s="111"/>
+      <c r="N24" s="111"/>
+      <c r="O24" s="111"/>
+      <c r="P24" s="111"/>
+      <c r="Q24" s="111"/>
+      <c r="R24" s="112"/>
     </row>
     <row r="25" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B25" s="89" t="s">
+      <c r="B25" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="90"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="90"/>
-      <c r="H25" s="90"/>
-      <c r="I25" s="90"/>
-      <c r="J25" s="90"/>
-      <c r="K25" s="90"/>
-      <c r="L25" s="90"/>
-      <c r="M25" s="90"/>
-      <c r="N25" s="90"/>
-      <c r="O25" s="90"/>
-      <c r="P25" s="90"/>
-      <c r="Q25" s="90"/>
-      <c r="R25" s="91"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="91"/>
+      <c r="H25" s="91"/>
+      <c r="I25" s="91"/>
+      <c r="J25" s="91"/>
+      <c r="K25" s="91"/>
+      <c r="L25" s="91"/>
+      <c r="M25" s="91"/>
+      <c r="N25" s="91"/>
+      <c r="O25" s="91"/>
+      <c r="P25" s="91"/>
+      <c r="Q25" s="91"/>
+      <c r="R25" s="92"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="R26" s="2"/>
@@ -4625,13 +4631,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="C1AqtvqKb8C414s7lEoNpdJ58hWR+bz87IU733aDeZMTPECU7crf3JYNQw8QcQksZnMw+dDwa8mNa2TsA5r9Aw==" saltValue="4/m+8HEyihP2IsZnh8JafA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="16">
-    <mergeCell ref="B10:R10"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B9:R9"/>
-    <mergeCell ref="B12:R12"/>
-    <mergeCell ref="B7:R7"/>
-    <mergeCell ref="B11:R11"/>
-    <mergeCell ref="B13:R13"/>
     <mergeCell ref="B22:R22"/>
     <mergeCell ref="B23:R23"/>
     <mergeCell ref="B25:R25"/>
@@ -4641,6 +4640,13 @@
     <mergeCell ref="B18:R18"/>
     <mergeCell ref="B19:R19"/>
     <mergeCell ref="B24:R24"/>
+    <mergeCell ref="B10:R10"/>
+    <mergeCell ref="B14:R14"/>
+    <mergeCell ref="B9:R9"/>
+    <mergeCell ref="B12:R12"/>
+    <mergeCell ref="B7:R7"/>
+    <mergeCell ref="B11:R11"/>
+    <mergeCell ref="B13:R13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -10529,8 +10535,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:R202"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H98" sqref="H98"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10627,7 +10633,7 @@
       </c>
       <c r="J4" s="41">
         <f>I202</f>
-        <v>412.49999999982538</v>
+        <v>422.49999999976717</v>
       </c>
       <c r="L4" s="133"/>
       <c r="R4" t="s">
@@ -10646,7 +10652,7 @@
       </c>
       <c r="J5" s="41">
         <f>J3-J4</f>
-        <v>1130.5000000001746</v>
+        <v>1120.5000000002328</v>
       </c>
       <c r="L5" s="133"/>
       <c r="M5" s="32"/>
@@ -13206,51 +13212,87 @@
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B98" s="9"/>
-      <c r="C98" s="9"/>
-      <c r="D98" s="9"/>
-      <c r="E98" s="82" t="str">
+      <c r="B98" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="E98" s="82">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="F98" s="12"/>
-      <c r="G98" s="12"/>
-      <c r="H98" s="11"/>
-      <c r="I98" s="36" t="str">
+        <v>239.99999999650754</v>
+      </c>
+      <c r="F98" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G98" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="H98" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I98" s="36">
         <f t="shared" si="3"/>
-        <v/>
+        <v>3.9999999999417923</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B99" s="9"/>
-      <c r="C99" s="9"/>
-      <c r="D99" s="9"/>
-      <c r="E99" s="82" t="str">
+      <c r="B99" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="E99" s="82">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="F99" s="12"/>
-      <c r="G99" s="12"/>
-      <c r="H99" s="11"/>
-      <c r="I99" s="36" t="str">
+        <v>180</v>
+      </c>
+      <c r="F99" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="H99" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I99" s="36">
         <f t="shared" si="3"/>
-        <v/>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B100" s="9"/>
-      <c r="C100" s="9"/>
-      <c r="D100" s="9"/>
-      <c r="E100" s="82" t="str">
+      <c r="B100" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="E100" s="82">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="F100" s="12"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="11"/>
-      <c r="I100" s="36" t="str">
+        <v>180</v>
+      </c>
+      <c r="F100" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G100" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="H100" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I100" s="36">
         <f t="shared" si="3"/>
-        <v/>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
@@ -14881,7 +14923,7 @@
       <c r="H202" s="35"/>
       <c r="I202" s="83">
         <f>SUM($I$8:I201)</f>
-        <v>412.49999999982538</v>
+        <v>422.49999999976717</v>
       </c>
     </row>
   </sheetData>
@@ -78553,12 +78595,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -78791,15 +78830,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5ECEC2-D611-47E4-BF40-446047C7D564}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E15B46B-DB71-477E-9F64-462B1A7F47C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -78824,10 +78867,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E15B46B-DB71-477E-9F64-462B1A7F47C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5ECEC2-D611-47E4-BF40-446047C7D564}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Finished ITPM Task 1, started task 2
</commit_message>
<xml_diff>
--- a/Off The Job Calculator - Joshua Morton.xlsx
+++ b/Off The Job Calculator - Joshua Morton.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoshMorton\Documents\_Degree\DegreePub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD8A521-45F7-4C8C-A841-899BB458D327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE17E0F-6593-4066-AE4A-B07B8234FC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66105" yWindow="540" windowWidth="28800" windowHeight="15285" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67050" yWindow="1980" windowWidth="28800" windowHeight="15285" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="4" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11242" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11260" uniqueCount="497">
   <si>
     <t>How to complete this calculator</t>
   </si>
@@ -1654,6 +1654,15 @@
   <si>
     <t>18/02/2024</t>
   </si>
+  <si>
+    <t>21/02/2024</t>
+  </si>
+  <si>
+    <t>22/02/2024</t>
+  </si>
+  <si>
+    <t>22/2/2024</t>
+  </si>
 </sst>
 </file>
 
@@ -2456,11 +2465,45 @@
     <xf numFmtId="49" fontId="15" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2487,40 +2530,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3715,9 +3724,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>326709</xdr:colOff>
+      <xdr:colOff>322899</xdr:colOff>
       <xdr:row>209</xdr:row>
-      <xdr:rowOff>59849</xdr:rowOff>
+      <xdr:rowOff>56039</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3764,9 +3773,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2078357</xdr:colOff>
+      <xdr:colOff>2074547</xdr:colOff>
       <xdr:row>208</xdr:row>
-      <xdr:rowOff>94774</xdr:rowOff>
+      <xdr:rowOff>98584</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3820,9 +3829,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>323374</xdr:colOff>
+      <xdr:colOff>327184</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>135660</xdr:rowOff>
+      <xdr:rowOff>131850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3863,9 +3872,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1583373</xdr:colOff>
+      <xdr:colOff>1579563</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>132485</xdr:rowOff>
+      <xdr:rowOff>136295</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3906,9 +3915,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>859029</xdr:colOff>
+      <xdr:colOff>855219</xdr:colOff>
       <xdr:row>208</xdr:row>
-      <xdr:rowOff>18256</xdr:rowOff>
+      <xdr:rowOff>22066</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4240,25 +4249,25 @@
   <sheetData>
     <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:18" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
-      <c r="J7" s="108"/>
-      <c r="K7" s="108"/>
-      <c r="L7" s="108"/>
-      <c r="M7" s="108"/>
-      <c r="N7" s="108"/>
-      <c r="O7" s="108"/>
-      <c r="P7" s="108"/>
-      <c r="Q7" s="108"/>
-      <c r="R7" s="109"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="99"/>
+      <c r="N7" s="99"/>
+      <c r="O7" s="99"/>
+      <c r="P7" s="99"/>
+      <c r="Q7" s="99"/>
+      <c r="R7" s="100"/>
     </row>
     <row r="8" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
@@ -4280,135 +4289,135 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B9" s="104" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="105"/>
-      <c r="H9" s="105"/>
-      <c r="I9" s="105"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="105"/>
-      <c r="L9" s="105"/>
-      <c r="M9" s="105"/>
-      <c r="N9" s="105"/>
-      <c r="O9" s="105"/>
-      <c r="P9" s="105"/>
-      <c r="Q9" s="105"/>
-      <c r="R9" s="105"/>
+      <c r="B9" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="94"/>
+      <c r="K9" s="94"/>
+      <c r="L9" s="94"/>
+      <c r="M9" s="94"/>
+      <c r="N9" s="94"/>
+      <c r="O9" s="94"/>
+      <c r="P9" s="94"/>
+      <c r="Q9" s="94"/>
+      <c r="R9" s="94"/>
     </row>
     <row r="10" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
-      <c r="B10" s="101" t="s">
+      <c r="B10" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="102"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="102"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102"/>
-      <c r="K10" s="102"/>
-      <c r="L10" s="102"/>
-      <c r="M10" s="102"/>
-      <c r="N10" s="102"/>
-      <c r="O10" s="102"/>
-      <c r="P10" s="102"/>
-      <c r="Q10" s="102"/>
-      <c r="R10" s="103"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="88"/>
+      <c r="L10" s="88"/>
+      <c r="M10" s="88"/>
+      <c r="N10" s="88"/>
+      <c r="O10" s="88"/>
+      <c r="P10" s="88"/>
+      <c r="Q10" s="88"/>
+      <c r="R10" s="89"/>
     </row>
     <row r="11" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="102"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="102"/>
-      <c r="M11" s="102"/>
-      <c r="N11" s="102"/>
-      <c r="O11" s="102"/>
-      <c r="P11" s="102"/>
-      <c r="Q11" s="102"/>
-      <c r="R11" s="103"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="88"/>
+      <c r="M11" s="88"/>
+      <c r="N11" s="88"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="88"/>
+      <c r="Q11" s="88"/>
+      <c r="R11" s="89"/>
     </row>
     <row r="12" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
-      <c r="B12" s="106" t="s">
+      <c r="B12" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="87"/>
-      <c r="M12" s="87"/>
-      <c r="N12" s="87"/>
-      <c r="O12" s="87"/>
-      <c r="P12" s="87"/>
-      <c r="Q12" s="87"/>
-      <c r="R12" s="88"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="96"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="96"/>
+      <c r="M12" s="96"/>
+      <c r="N12" s="96"/>
+      <c r="O12" s="96"/>
+      <c r="P12" s="96"/>
+      <c r="Q12" s="96"/>
+      <c r="R12" s="97"/>
     </row>
     <row r="13" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
-      <c r="B13" s="110" t="s">
+      <c r="B13" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
-      <c r="L13" s="111"/>
-      <c r="M13" s="111"/>
-      <c r="N13" s="111"/>
-      <c r="O13" s="111"/>
-      <c r="P13" s="111"/>
-      <c r="Q13" s="111"/>
-      <c r="R13" s="112"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
+      <c r="O13" s="102"/>
+      <c r="P13" s="102"/>
+      <c r="Q13" s="102"/>
+      <c r="R13" s="103"/>
     </row>
     <row r="14" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
-      <c r="B14" s="89" t="s">
+      <c r="B14" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
-      <c r="K14" s="90"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="90"/>
-      <c r="O14" s="90"/>
-      <c r="P14" s="90"/>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="91"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="91"/>
+      <c r="K14" s="91"/>
+      <c r="L14" s="91"/>
+      <c r="M14" s="91"/>
+      <c r="N14" s="91"/>
+      <c r="O14" s="91"/>
+      <c r="P14" s="91"/>
+      <c r="Q14" s="91"/>
+      <c r="R14" s="92"/>
     </row>
     <row r="15" spans="1:18" ht="5.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
@@ -4430,91 +4439,91 @@
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="93"/>
-      <c r="K16" s="93"/>
-      <c r="L16" s="93"/>
-      <c r="M16" s="93"/>
-      <c r="N16" s="93"/>
-      <c r="O16" s="93"/>
-      <c r="P16" s="93"/>
-      <c r="Q16" s="93"/>
-      <c r="R16" s="93"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="105"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="105"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="105"/>
+      <c r="N16" s="105"/>
+      <c r="O16" s="105"/>
+      <c r="P16" s="105"/>
+      <c r="Q16" s="105"/>
+      <c r="R16" s="105"/>
     </row>
     <row r="17" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A17" s="2"/>
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="87"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="87"/>
-      <c r="K17" s="87"/>
-      <c r="L17" s="87"/>
-      <c r="M17" s="87"/>
-      <c r="N17" s="87"/>
-      <c r="O17" s="87"/>
-      <c r="P17" s="87"/>
-      <c r="Q17" s="87"/>
-      <c r="R17" s="88"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="96"/>
+      <c r="M17" s="96"/>
+      <c r="N17" s="96"/>
+      <c r="O17" s="96"/>
+      <c r="P17" s="96"/>
+      <c r="Q17" s="96"/>
+      <c r="R17" s="97"/>
     </row>
     <row r="18" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
-      <c r="B18" s="87" t="s">
+      <c r="B18" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="87"/>
-      <c r="K18" s="87"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87"/>
-      <c r="O18" s="87"/>
-      <c r="P18" s="87"/>
-      <c r="Q18" s="87"/>
-      <c r="R18" s="88"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="96"/>
+      <c r="J18" s="96"/>
+      <c r="K18" s="96"/>
+      <c r="L18" s="96"/>
+      <c r="M18" s="96"/>
+      <c r="N18" s="96"/>
+      <c r="O18" s="96"/>
+      <c r="P18" s="96"/>
+      <c r="Q18" s="96"/>
+      <c r="R18" s="97"/>
     </row>
     <row r="19" spans="1:18" ht="32.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="96"/>
-      <c r="I19" s="96"/>
-      <c r="J19" s="96"/>
-      <c r="K19" s="96"/>
-      <c r="L19" s="96"/>
-      <c r="M19" s="96"/>
-      <c r="N19" s="96"/>
-      <c r="O19" s="96"/>
-      <c r="P19" s="96"/>
-      <c r="Q19" s="96"/>
-      <c r="R19" s="97"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="108"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="108"/>
+      <c r="J19" s="108"/>
+      <c r="K19" s="108"/>
+      <c r="L19" s="108"/>
+      <c r="M19" s="108"/>
+      <c r="N19" s="108"/>
+      <c r="O19" s="108"/>
+      <c r="P19" s="108"/>
+      <c r="Q19" s="108"/>
+      <c r="R19" s="109"/>
     </row>
     <row r="20" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="3"/>
@@ -4536,112 +4545,112 @@
       <c r="R20" s="5"/>
     </row>
     <row r="21" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="95"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="95"/>
-      <c r="G21" s="95"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="95"/>
-      <c r="J21" s="95"/>
-      <c r="K21" s="95"/>
-      <c r="L21" s="95"/>
-      <c r="M21" s="95"/>
-      <c r="N21" s="95"/>
-      <c r="O21" s="95"/>
-      <c r="P21" s="95"/>
-      <c r="Q21" s="95"/>
-      <c r="R21" s="95"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="107"/>
+      <c r="E21" s="107"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="107"/>
+      <c r="I21" s="107"/>
+      <c r="J21" s="107"/>
+      <c r="K21" s="107"/>
+      <c r="L21" s="107"/>
+      <c r="M21" s="107"/>
+      <c r="N21" s="107"/>
+      <c r="O21" s="107"/>
+      <c r="P21" s="107"/>
+      <c r="Q21" s="107"/>
+      <c r="R21" s="107"/>
     </row>
     <row r="22" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A22" s="2"/>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="87"/>
-      <c r="J22" s="87"/>
-      <c r="K22" s="87"/>
-      <c r="L22" s="87"/>
-      <c r="M22" s="87"/>
-      <c r="N22" s="87"/>
-      <c r="O22" s="87"/>
-      <c r="P22" s="87"/>
-      <c r="Q22" s="87"/>
-      <c r="R22" s="88"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="96"/>
+      <c r="J22" s="96"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="96"/>
+      <c r="O22" s="96"/>
+      <c r="P22" s="96"/>
+      <c r="Q22" s="96"/>
+      <c r="R22" s="97"/>
     </row>
     <row r="23" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="87"/>
-      <c r="K23" s="87"/>
-      <c r="L23" s="87"/>
-      <c r="M23" s="87"/>
-      <c r="N23" s="87"/>
-      <c r="O23" s="87"/>
-      <c r="P23" s="87"/>
-      <c r="Q23" s="87"/>
-      <c r="R23" s="88"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="96"/>
+      <c r="P23" s="96"/>
+      <c r="Q23" s="96"/>
+      <c r="R23" s="97"/>
     </row>
     <row r="24" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A24" s="2"/>
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="99"/>
-      <c r="D24" s="99"/>
-      <c r="E24" s="99"/>
-      <c r="F24" s="99"/>
-      <c r="G24" s="99"/>
-      <c r="H24" s="99"/>
-      <c r="I24" s="99"/>
-      <c r="J24" s="99"/>
-      <c r="K24" s="99"/>
-      <c r="L24" s="99"/>
-      <c r="M24" s="99"/>
-      <c r="N24" s="99"/>
-      <c r="O24" s="99"/>
-      <c r="P24" s="99"/>
-      <c r="Q24" s="99"/>
-      <c r="R24" s="100"/>
+      <c r="C24" s="111"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="111"/>
+      <c r="G24" s="111"/>
+      <c r="H24" s="111"/>
+      <c r="I24" s="111"/>
+      <c r="J24" s="111"/>
+      <c r="K24" s="111"/>
+      <c r="L24" s="111"/>
+      <c r="M24" s="111"/>
+      <c r="N24" s="111"/>
+      <c r="O24" s="111"/>
+      <c r="P24" s="111"/>
+      <c r="Q24" s="111"/>
+      <c r="R24" s="112"/>
     </row>
     <row r="25" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B25" s="89" t="s">
+      <c r="B25" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="90"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="90"/>
-      <c r="H25" s="90"/>
-      <c r="I25" s="90"/>
-      <c r="J25" s="90"/>
-      <c r="K25" s="90"/>
-      <c r="L25" s="90"/>
-      <c r="M25" s="90"/>
-      <c r="N25" s="90"/>
-      <c r="O25" s="90"/>
-      <c r="P25" s="90"/>
-      <c r="Q25" s="90"/>
-      <c r="R25" s="91"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="91"/>
+      <c r="H25" s="91"/>
+      <c r="I25" s="91"/>
+      <c r="J25" s="91"/>
+      <c r="K25" s="91"/>
+      <c r="L25" s="91"/>
+      <c r="M25" s="91"/>
+      <c r="N25" s="91"/>
+      <c r="O25" s="91"/>
+      <c r="P25" s="91"/>
+      <c r="Q25" s="91"/>
+      <c r="R25" s="92"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="R26" s="2"/>
@@ -4649,13 +4658,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="C1AqtvqKb8C414s7lEoNpdJ58hWR+bz87IU733aDeZMTPECU7crf3JYNQw8QcQksZnMw+dDwa8mNa2TsA5r9Aw==" saltValue="4/m+8HEyihP2IsZnh8JafA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="16">
-    <mergeCell ref="B10:R10"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B9:R9"/>
-    <mergeCell ref="B12:R12"/>
-    <mergeCell ref="B7:R7"/>
-    <mergeCell ref="B11:R11"/>
-    <mergeCell ref="B13:R13"/>
     <mergeCell ref="B22:R22"/>
     <mergeCell ref="B23:R23"/>
     <mergeCell ref="B25:R25"/>
@@ -4665,6 +4667,13 @@
     <mergeCell ref="B18:R18"/>
     <mergeCell ref="B19:R19"/>
     <mergeCell ref="B24:R24"/>
+    <mergeCell ref="B10:R10"/>
+    <mergeCell ref="B14:R14"/>
+    <mergeCell ref="B9:R9"/>
+    <mergeCell ref="B12:R12"/>
+    <mergeCell ref="B7:R7"/>
+    <mergeCell ref="B11:R11"/>
+    <mergeCell ref="B13:R13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -10554,7 +10563,7 @@
   <dimension ref="B1:R202"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H107" sqref="H107"/>
+      <selection activeCell="H110" sqref="H110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10651,7 +10660,7 @@
       </c>
       <c r="J4" s="41">
         <f>I202</f>
-        <v>448.99999999970896</v>
+        <v>459.99999999976717</v>
       </c>
       <c r="L4" s="133"/>
       <c r="R4" t="s">
@@ -10670,7 +10679,7 @@
       </c>
       <c r="J5" s="41">
         <f>J3-J4</f>
-        <v>1094.000000000291</v>
+        <v>1083.0000000002328</v>
       </c>
       <c r="L5" s="133"/>
       <c r="M5" s="32"/>
@@ -13482,51 +13491,87 @@
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B107" s="9"/>
-      <c r="C107" s="9"/>
-      <c r="D107" s="9"/>
-      <c r="E107" s="82" t="str">
+      <c r="B107" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="E107" s="82">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="F107" s="12"/>
-      <c r="G107" s="12"/>
-      <c r="H107" s="11"/>
-      <c r="I107" s="36" t="str">
+        <v>180</v>
+      </c>
+      <c r="F107" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G107" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="H107" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I107" s="36">
         <f t="shared" si="3"/>
-        <v/>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B108" s="9"/>
-      <c r="C108" s="9"/>
-      <c r="D108" s="9"/>
-      <c r="E108" s="82" t="str">
+      <c r="B108" s="9" t="s">
+        <v>495</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="E108" s="82">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="F108" s="12"/>
-      <c r="G108" s="12"/>
-      <c r="H108" s="11"/>
-      <c r="I108" s="36" t="str">
+        <v>180</v>
+      </c>
+      <c r="F108" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G108" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="H108" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="I108" s="36">
         <f t="shared" si="3"/>
-        <v/>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B109" s="9"/>
-      <c r="C109" s="9"/>
-      <c r="D109" s="9"/>
-      <c r="E109" s="82" t="str">
+      <c r="B109" s="9" t="s">
+        <v>496</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="D109" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="E109" s="82">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="F109" s="12"/>
-      <c r="G109" s="12"/>
-      <c r="H109" s="11"/>
-      <c r="I109" s="36" t="str">
+        <v>300.00000000349246</v>
+      </c>
+      <c r="F109" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G109" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="H109" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I109" s="36">
         <f t="shared" si="3"/>
-        <v/>
+        <v>5.0000000000582077</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.3">
@@ -15013,7 +15058,7 @@
       <c r="H202" s="35"/>
       <c r="I202" s="83">
         <f>SUM($I$8:I201)</f>
-        <v>448.99999999970896</v>
+        <v>459.99999999976717</v>
       </c>
     </row>
   </sheetData>
@@ -78685,12 +78730,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -78923,15 +78965,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5ECEC2-D611-47E4-BF40-446047C7D564}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E15B46B-DB71-477E-9F64-462B1A7F47C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -78956,10 +79002,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E15B46B-DB71-477E-9F64-462B1A7F47C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5ECEC2-D611-47E4-BF40-446047C7D564}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Stage 2 Draft 1 finito + otjc
</commit_message>
<xml_diff>
--- a/Off The Job Calculator - Joshua Morton.xlsx
+++ b/Off The Job Calculator - Joshua Morton.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoshMorton\Documents\_Degree\DegreePub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE17E0F-6593-4066-AE4A-B07B8234FC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F51544-262A-4604-9407-0EE366AECA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67050" yWindow="1980" windowWidth="28800" windowHeight="15285" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="4" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11260" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11266" uniqueCount="497">
   <si>
     <t>How to complete this calculator</t>
   </si>
@@ -1661,7 +1661,7 @@
     <t>22/02/2024</t>
   </si>
   <si>
-    <t>22/2/2024</t>
+    <t>26/02/2024</t>
   </si>
 </sst>
 </file>
@@ -2465,45 +2465,11 @@
     <xf numFmtId="49" fontId="15" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2530,6 +2496,40 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3724,9 +3724,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>322899</xdr:colOff>
+      <xdr:colOff>326709</xdr:colOff>
       <xdr:row>209</xdr:row>
-      <xdr:rowOff>56039</xdr:rowOff>
+      <xdr:rowOff>59849</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3773,9 +3773,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2074547</xdr:colOff>
+      <xdr:colOff>2078357</xdr:colOff>
       <xdr:row>208</xdr:row>
-      <xdr:rowOff>98584</xdr:rowOff>
+      <xdr:rowOff>94774</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3829,9 +3829,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>327184</xdr:colOff>
+      <xdr:colOff>323374</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>131850</xdr:rowOff>
+      <xdr:rowOff>135660</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3872,9 +3872,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1579563</xdr:colOff>
+      <xdr:colOff>1583373</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>136295</xdr:rowOff>
+      <xdr:rowOff>132485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3915,9 +3915,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>855219</xdr:colOff>
+      <xdr:colOff>859029</xdr:colOff>
       <xdr:row>208</xdr:row>
-      <xdr:rowOff>22066</xdr:rowOff>
+      <xdr:rowOff>18256</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4249,25 +4249,25 @@
   <sheetData>
     <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:18" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
-      <c r="N7" s="99"/>
-      <c r="O7" s="99"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="99"/>
-      <c r="R7" s="100"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="108"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="108"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="108"/>
+      <c r="R7" s="109"/>
     </row>
     <row r="8" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
@@ -4289,135 +4289,135 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B9" s="93" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="94"/>
-      <c r="O9" s="94"/>
-      <c r="P9" s="94"/>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="94"/>
+      <c r="B9" s="104" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="105"/>
+      <c r="M9" s="105"/>
+      <c r="N9" s="105"/>
+      <c r="O9" s="105"/>
+      <c r="P9" s="105"/>
+      <c r="Q9" s="105"/>
+      <c r="R9" s="105"/>
     </row>
     <row r="10" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
-      <c r="B10" s="87" t="s">
+      <c r="B10" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
-      <c r="L10" s="88"/>
-      <c r="M10" s="88"/>
-      <c r="N10" s="88"/>
-      <c r="O10" s="88"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="89"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="102"/>
+      <c r="I10" s="102"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="102"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
+      <c r="O10" s="102"/>
+      <c r="P10" s="102"/>
+      <c r="Q10" s="102"/>
+      <c r="R10" s="103"/>
     </row>
     <row r="11" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="88"/>
-      <c r="L11" s="88"/>
-      <c r="M11" s="88"/>
-      <c r="N11" s="88"/>
-      <c r="O11" s="88"/>
-      <c r="P11" s="88"/>
-      <c r="Q11" s="88"/>
-      <c r="R11" s="89"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="102"/>
+      <c r="N11" s="102"/>
+      <c r="O11" s="102"/>
+      <c r="P11" s="102"/>
+      <c r="Q11" s="102"/>
+      <c r="R11" s="103"/>
     </row>
     <row r="12" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
-      <c r="B12" s="95" t="s">
+      <c r="B12" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="96"/>
-      <c r="F12" s="96"/>
-      <c r="G12" s="96"/>
-      <c r="H12" s="96"/>
-      <c r="I12" s="96"/>
-      <c r="J12" s="96"/>
-      <c r="K12" s="96"/>
-      <c r="L12" s="96"/>
-      <c r="M12" s="96"/>
-      <c r="N12" s="96"/>
-      <c r="O12" s="96"/>
-      <c r="P12" s="96"/>
-      <c r="Q12" s="96"/>
-      <c r="R12" s="97"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="88"/>
     </row>
     <row r="13" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="102"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="102"/>
-      <c r="L13" s="102"/>
-      <c r="M13" s="102"/>
-      <c r="N13" s="102"/>
-      <c r="O13" s="102"/>
-      <c r="P13" s="102"/>
-      <c r="Q13" s="102"/>
-      <c r="R13" s="103"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="111"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="111"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="111"/>
+      <c r="R13" s="112"/>
     </row>
     <row r="14" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="91"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="91"/>
-      <c r="K14" s="91"/>
-      <c r="L14" s="91"/>
-      <c r="M14" s="91"/>
-      <c r="N14" s="91"/>
-      <c r="O14" s="91"/>
-      <c r="P14" s="91"/>
-      <c r="Q14" s="91"/>
-      <c r="R14" s="92"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="90"/>
+      <c r="M14" s="90"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="90"/>
+      <c r="P14" s="90"/>
+      <c r="Q14" s="90"/>
+      <c r="R14" s="91"/>
     </row>
     <row r="15" spans="1:18" ht="5.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
@@ -4439,91 +4439,91 @@
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B16" s="104" t="s">
+      <c r="B16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="105"/>
-      <c r="K16" s="105"/>
-      <c r="L16" s="105"/>
-      <c r="M16" s="105"/>
-      <c r="N16" s="105"/>
-      <c r="O16" s="105"/>
-      <c r="P16" s="105"/>
-      <c r="Q16" s="105"/>
-      <c r="R16" s="105"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="93"/>
+      <c r="M16" s="93"/>
+      <c r="N16" s="93"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="93"/>
     </row>
     <row r="17" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A17" s="2"/>
-      <c r="B17" s="96" t="s">
+      <c r="B17" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="97"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="87"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="87"/>
+      <c r="O17" s="87"/>
+      <c r="P17" s="87"/>
+      <c r="Q17" s="87"/>
+      <c r="R17" s="88"/>
     </row>
     <row r="18" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="96"/>
-      <c r="J18" s="96"/>
-      <c r="K18" s="96"/>
-      <c r="L18" s="96"/>
-      <c r="M18" s="96"/>
-      <c r="N18" s="96"/>
-      <c r="O18" s="96"/>
-      <c r="P18" s="96"/>
-      <c r="Q18" s="96"/>
-      <c r="R18" s="97"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="87"/>
+      <c r="M18" s="87"/>
+      <c r="N18" s="87"/>
+      <c r="O18" s="87"/>
+      <c r="P18" s="87"/>
+      <c r="Q18" s="87"/>
+      <c r="R18" s="88"/>
     </row>
     <row r="19" spans="1:18" ht="32.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="108"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="108"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="108"/>
-      <c r="K19" s="108"/>
-      <c r="L19" s="108"/>
-      <c r="M19" s="108"/>
-      <c r="N19" s="108"/>
-      <c r="O19" s="108"/>
-      <c r="P19" s="108"/>
-      <c r="Q19" s="108"/>
-      <c r="R19" s="109"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="96"/>
+      <c r="I19" s="96"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="96"/>
+      <c r="L19" s="96"/>
+      <c r="M19" s="96"/>
+      <c r="N19" s="96"/>
+      <c r="O19" s="96"/>
+      <c r="P19" s="96"/>
+      <c r="Q19" s="96"/>
+      <c r="R19" s="97"/>
     </row>
     <row r="20" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="3"/>
@@ -4545,112 +4545,112 @@
       <c r="R20" s="5"/>
     </row>
     <row r="21" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B21" s="106" t="s">
+      <c r="B21" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="107"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="107"/>
-      <c r="H21" s="107"/>
-      <c r="I21" s="107"/>
-      <c r="J21" s="107"/>
-      <c r="K21" s="107"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="107"/>
-      <c r="N21" s="107"/>
-      <c r="O21" s="107"/>
-      <c r="P21" s="107"/>
-      <c r="Q21" s="107"/>
-      <c r="R21" s="107"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="95"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="95"/>
+      <c r="K21" s="95"/>
+      <c r="L21" s="95"/>
+      <c r="M21" s="95"/>
+      <c r="N21" s="95"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="95"/>
+      <c r="R21" s="95"/>
     </row>
     <row r="22" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A22" s="2"/>
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="96"/>
-      <c r="I22" s="96"/>
-      <c r="J22" s="96"/>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="96"/>
-      <c r="O22" s="96"/>
-      <c r="P22" s="96"/>
-      <c r="Q22" s="96"/>
-      <c r="R22" s="97"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="87"/>
+      <c r="M22" s="87"/>
+      <c r="N22" s="87"/>
+      <c r="O22" s="87"/>
+      <c r="P22" s="87"/>
+      <c r="Q22" s="87"/>
+      <c r="R22" s="88"/>
     </row>
     <row r="23" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
-      <c r="B23" s="96" t="s">
+      <c r="B23" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="96"/>
-      <c r="I23" s="96"/>
-      <c r="J23" s="96"/>
-      <c r="K23" s="96"/>
-      <c r="L23" s="96"/>
-      <c r="M23" s="96"/>
-      <c r="N23" s="96"/>
-      <c r="O23" s="96"/>
-      <c r="P23" s="96"/>
-      <c r="Q23" s="96"/>
-      <c r="R23" s="97"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="87"/>
+      <c r="J23" s="87"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="87"/>
+      <c r="M23" s="87"/>
+      <c r="N23" s="87"/>
+      <c r="O23" s="87"/>
+      <c r="P23" s="87"/>
+      <c r="Q23" s="87"/>
+      <c r="R23" s="88"/>
     </row>
     <row r="24" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A24" s="2"/>
-      <c r="B24" s="110" t="s">
+      <c r="B24" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="111"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="111"/>
-      <c r="H24" s="111"/>
-      <c r="I24" s="111"/>
-      <c r="J24" s="111"/>
-      <c r="K24" s="111"/>
-      <c r="L24" s="111"/>
-      <c r="M24" s="111"/>
-      <c r="N24" s="111"/>
-      <c r="O24" s="111"/>
-      <c r="P24" s="111"/>
-      <c r="Q24" s="111"/>
-      <c r="R24" s="112"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="99"/>
+      <c r="J24" s="99"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="99"/>
+      <c r="M24" s="99"/>
+      <c r="N24" s="99"/>
+      <c r="O24" s="99"/>
+      <c r="P24" s="99"/>
+      <c r="Q24" s="99"/>
+      <c r="R24" s="100"/>
     </row>
     <row r="25" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B25" s="90" t="s">
+      <c r="B25" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="91"/>
-      <c r="I25" s="91"/>
-      <c r="J25" s="91"/>
-      <c r="K25" s="91"/>
-      <c r="L25" s="91"/>
-      <c r="M25" s="91"/>
-      <c r="N25" s="91"/>
-      <c r="O25" s="91"/>
-      <c r="P25" s="91"/>
-      <c r="Q25" s="91"/>
-      <c r="R25" s="92"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="90"/>
+      <c r="H25" s="90"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="90"/>
+      <c r="N25" s="90"/>
+      <c r="O25" s="90"/>
+      <c r="P25" s="90"/>
+      <c r="Q25" s="90"/>
+      <c r="R25" s="91"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="R26" s="2"/>
@@ -4658,6 +4658,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="C1AqtvqKb8C414s7lEoNpdJ58hWR+bz87IU733aDeZMTPECU7crf3JYNQw8QcQksZnMw+dDwa8mNa2TsA5r9Aw==" saltValue="4/m+8HEyihP2IsZnh8JafA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="16">
+    <mergeCell ref="B10:R10"/>
+    <mergeCell ref="B14:R14"/>
+    <mergeCell ref="B9:R9"/>
+    <mergeCell ref="B12:R12"/>
+    <mergeCell ref="B7:R7"/>
+    <mergeCell ref="B11:R11"/>
+    <mergeCell ref="B13:R13"/>
     <mergeCell ref="B22:R22"/>
     <mergeCell ref="B23:R23"/>
     <mergeCell ref="B25:R25"/>
@@ -4667,13 +4674,6 @@
     <mergeCell ref="B18:R18"/>
     <mergeCell ref="B19:R19"/>
     <mergeCell ref="B24:R24"/>
-    <mergeCell ref="B10:R10"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B9:R9"/>
-    <mergeCell ref="B12:R12"/>
-    <mergeCell ref="B7:R7"/>
-    <mergeCell ref="B11:R11"/>
-    <mergeCell ref="B13:R13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -10563,7 +10563,7 @@
   <dimension ref="B1:R202"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+      <selection activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10660,7 +10660,7 @@
       </c>
       <c r="J4" s="41">
         <f>I202</f>
-        <v>459.99999999976717</v>
+        <v>463.99999999970896</v>
       </c>
       <c r="L4" s="133"/>
       <c r="R4" t="s">
@@ -10679,7 +10679,7 @@
       </c>
       <c r="J5" s="41">
         <f>J3-J4</f>
-        <v>1083.0000000002328</v>
+        <v>1079.000000000291</v>
       </c>
       <c r="L5" s="133"/>
       <c r="M5" s="32"/>
@@ -13548,7 +13548,7 @@
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B109" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C109" s="9" t="s">
         <v>359</v>
@@ -13575,19 +13575,31 @@
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B110" s="9"/>
-      <c r="C110" s="9"/>
-      <c r="D110" s="9"/>
-      <c r="E110" s="82" t="str">
+      <c r="B110" s="9" t="s">
+        <v>496</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="D110" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="E110" s="82">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="F110" s="12"/>
-      <c r="G110" s="12"/>
-      <c r="H110" s="11"/>
-      <c r="I110" s="36" t="str">
+        <v>239.99999999650754</v>
+      </c>
+      <c r="F110" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G110" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="H110" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I110" s="36">
         <f t="shared" si="3"/>
-        <v/>
+        <v>3.9999999999417923</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
@@ -15058,7 +15070,7 @@
       <c r="H202" s="35"/>
       <c r="I202" s="83">
         <f>SUM($I$8:I201)</f>
-        <v>459.99999999976717</v>
+        <v>463.99999999970896</v>
       </c>
     </row>
   </sheetData>
@@ -78730,9 +78742,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -78965,19 +78980,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E15B46B-DB71-477E-9F64-462B1A7F47C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5ECEC2-D611-47E4-BF40-446047C7D564}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -79002,9 +79013,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5ECEC2-D611-47E4-BF40-446047C7D564}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E15B46B-DB71-477E-9F64-462B1A7F47C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Started to plan CSA
</commit_message>
<xml_diff>
--- a/Off The Job Calculator - Joshua Morton.xlsx
+++ b/Off The Job Calculator - Joshua Morton.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoshMorton\Documents\_Degree\DegreePub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F35CCE-ADC2-41AF-9F41-11F15ED65EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71760AA0-980F-4930-B771-D4FF925B15B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11470" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11518" uniqueCount="537">
   <si>
     <t>How to complete this calculator</t>
   </si>
@@ -1762,6 +1762,27 @@
   <si>
     <t>30/05/2024</t>
   </si>
+  <si>
+    <t>04/06/2024</t>
+  </si>
+  <si>
+    <t>05/06/2024</t>
+  </si>
+  <si>
+    <t>11/06/2024</t>
+  </si>
+  <si>
+    <t>14/06/2024</t>
+  </si>
+  <si>
+    <t>18/06/2024</t>
+  </si>
+  <si>
+    <t>20/06/2024</t>
+  </si>
+  <si>
+    <t>26/06/2024</t>
+  </si>
 </sst>
 </file>
 
@@ -2564,45 +2585,11 @@
     <xf numFmtId="49" fontId="15" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2629,6 +2616,40 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4348,25 +4369,25 @@
   <sheetData>
     <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:18" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
-      <c r="N7" s="99"/>
-      <c r="O7" s="99"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="99"/>
-      <c r="R7" s="100"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="108"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="108"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="108"/>
+      <c r="R7" s="109"/>
     </row>
     <row r="8" spans="1:18" ht="4.6500000000000004" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
@@ -4388,135 +4409,135 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B9" s="93" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="94"/>
-      <c r="O9" s="94"/>
-      <c r="P9" s="94"/>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="94"/>
+      <c r="B9" s="104" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="105"/>
+      <c r="M9" s="105"/>
+      <c r="N9" s="105"/>
+      <c r="O9" s="105"/>
+      <c r="P9" s="105"/>
+      <c r="Q9" s="105"/>
+      <c r="R9" s="105"/>
     </row>
     <row r="10" spans="1:18" ht="31.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
-      <c r="B10" s="87" t="s">
+      <c r="B10" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
-      <c r="L10" s="88"/>
-      <c r="M10" s="88"/>
-      <c r="N10" s="88"/>
-      <c r="O10" s="88"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="89"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="102"/>
+      <c r="I10" s="102"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="102"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
+      <c r="O10" s="102"/>
+      <c r="P10" s="102"/>
+      <c r="Q10" s="102"/>
+      <c r="R10" s="103"/>
     </row>
     <row r="11" spans="1:18" ht="31.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="88"/>
-      <c r="L11" s="88"/>
-      <c r="M11" s="88"/>
-      <c r="N11" s="88"/>
-      <c r="O11" s="88"/>
-      <c r="P11" s="88"/>
-      <c r="Q11" s="88"/>
-      <c r="R11" s="89"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="102"/>
+      <c r="N11" s="102"/>
+      <c r="O11" s="102"/>
+      <c r="P11" s="102"/>
+      <c r="Q11" s="102"/>
+      <c r="R11" s="103"/>
     </row>
     <row r="12" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
-      <c r="B12" s="95" t="s">
+      <c r="B12" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="96"/>
-      <c r="F12" s="96"/>
-      <c r="G12" s="96"/>
-      <c r="H12" s="96"/>
-      <c r="I12" s="96"/>
-      <c r="J12" s="96"/>
-      <c r="K12" s="96"/>
-      <c r="L12" s="96"/>
-      <c r="M12" s="96"/>
-      <c r="N12" s="96"/>
-      <c r="O12" s="96"/>
-      <c r="P12" s="96"/>
-      <c r="Q12" s="96"/>
-      <c r="R12" s="97"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="88"/>
     </row>
     <row r="13" spans="1:18" ht="31.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="102"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="102"/>
-      <c r="L13" s="102"/>
-      <c r="M13" s="102"/>
-      <c r="N13" s="102"/>
-      <c r="O13" s="102"/>
-      <c r="P13" s="102"/>
-      <c r="Q13" s="102"/>
-      <c r="R13" s="103"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="111"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="111"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="111"/>
+      <c r="R13" s="112"/>
     </row>
     <row r="14" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="91"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="91"/>
-      <c r="K14" s="91"/>
-      <c r="L14" s="91"/>
-      <c r="M14" s="91"/>
-      <c r="N14" s="91"/>
-      <c r="O14" s="91"/>
-      <c r="P14" s="91"/>
-      <c r="Q14" s="91"/>
-      <c r="R14" s="92"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="90"/>
+      <c r="M14" s="90"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="90"/>
+      <c r="P14" s="90"/>
+      <c r="Q14" s="90"/>
+      <c r="R14" s="91"/>
     </row>
     <row r="15" spans="1:18" ht="5.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
@@ -4538,91 +4559,91 @@
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B16" s="104" t="s">
+      <c r="B16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="105"/>
-      <c r="K16" s="105"/>
-      <c r="L16" s="105"/>
-      <c r="M16" s="105"/>
-      <c r="N16" s="105"/>
-      <c r="O16" s="105"/>
-      <c r="P16" s="105"/>
-      <c r="Q16" s="105"/>
-      <c r="R16" s="105"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="93"/>
+      <c r="M16" s="93"/>
+      <c r="N16" s="93"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="93"/>
     </row>
     <row r="17" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A17" s="2"/>
-      <c r="B17" s="96" t="s">
+      <c r="B17" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="97"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="87"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="87"/>
+      <c r="O17" s="87"/>
+      <c r="P17" s="87"/>
+      <c r="Q17" s="87"/>
+      <c r="R17" s="88"/>
     </row>
     <row r="18" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="96"/>
-      <c r="J18" s="96"/>
-      <c r="K18" s="96"/>
-      <c r="L18" s="96"/>
-      <c r="M18" s="96"/>
-      <c r="N18" s="96"/>
-      <c r="O18" s="96"/>
-      <c r="P18" s="96"/>
-      <c r="Q18" s="96"/>
-      <c r="R18" s="97"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="87"/>
+      <c r="M18" s="87"/>
+      <c r="N18" s="87"/>
+      <c r="O18" s="87"/>
+      <c r="P18" s="87"/>
+      <c r="Q18" s="87"/>
+      <c r="R18" s="88"/>
     </row>
     <row r="19" spans="1:18" ht="32.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="108"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="108"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="108"/>
-      <c r="K19" s="108"/>
-      <c r="L19" s="108"/>
-      <c r="M19" s="108"/>
-      <c r="N19" s="108"/>
-      <c r="O19" s="108"/>
-      <c r="P19" s="108"/>
-      <c r="Q19" s="108"/>
-      <c r="R19" s="109"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="96"/>
+      <c r="I19" s="96"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="96"/>
+      <c r="L19" s="96"/>
+      <c r="M19" s="96"/>
+      <c r="N19" s="96"/>
+      <c r="O19" s="96"/>
+      <c r="P19" s="96"/>
+      <c r="Q19" s="96"/>
+      <c r="R19" s="97"/>
     </row>
     <row r="20" spans="1:18" ht="4.6500000000000004" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="3"/>
@@ -4644,112 +4665,112 @@
       <c r="R20" s="5"/>
     </row>
     <row r="21" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B21" s="106" t="s">
+      <c r="B21" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="107"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="107"/>
-      <c r="H21" s="107"/>
-      <c r="I21" s="107"/>
-      <c r="J21" s="107"/>
-      <c r="K21" s="107"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="107"/>
-      <c r="N21" s="107"/>
-      <c r="O21" s="107"/>
-      <c r="P21" s="107"/>
-      <c r="Q21" s="107"/>
-      <c r="R21" s="107"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="95"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="95"/>
+      <c r="K21" s="95"/>
+      <c r="L21" s="95"/>
+      <c r="M21" s="95"/>
+      <c r="N21" s="95"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="95"/>
+      <c r="R21" s="95"/>
     </row>
     <row r="22" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A22" s="2"/>
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="96"/>
-      <c r="I22" s="96"/>
-      <c r="J22" s="96"/>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="96"/>
-      <c r="O22" s="96"/>
-      <c r="P22" s="96"/>
-      <c r="Q22" s="96"/>
-      <c r="R22" s="97"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="87"/>
+      <c r="M22" s="87"/>
+      <c r="N22" s="87"/>
+      <c r="O22" s="87"/>
+      <c r="P22" s="87"/>
+      <c r="Q22" s="87"/>
+      <c r="R22" s="88"/>
     </row>
     <row r="23" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
-      <c r="B23" s="96" t="s">
+      <c r="B23" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="96"/>
-      <c r="I23" s="96"/>
-      <c r="J23" s="96"/>
-      <c r="K23" s="96"/>
-      <c r="L23" s="96"/>
-      <c r="M23" s="96"/>
-      <c r="N23" s="96"/>
-      <c r="O23" s="96"/>
-      <c r="P23" s="96"/>
-      <c r="Q23" s="96"/>
-      <c r="R23" s="97"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="87"/>
+      <c r="J23" s="87"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="87"/>
+      <c r="M23" s="87"/>
+      <c r="N23" s="87"/>
+      <c r="O23" s="87"/>
+      <c r="P23" s="87"/>
+      <c r="Q23" s="87"/>
+      <c r="R23" s="88"/>
     </row>
     <row r="24" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A24" s="2"/>
-      <c r="B24" s="110" t="s">
+      <c r="B24" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="111"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="111"/>
-      <c r="H24" s="111"/>
-      <c r="I24" s="111"/>
-      <c r="J24" s="111"/>
-      <c r="K24" s="111"/>
-      <c r="L24" s="111"/>
-      <c r="M24" s="111"/>
-      <c r="N24" s="111"/>
-      <c r="O24" s="111"/>
-      <c r="P24" s="111"/>
-      <c r="Q24" s="111"/>
-      <c r="R24" s="112"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="99"/>
+      <c r="J24" s="99"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="99"/>
+      <c r="M24" s="99"/>
+      <c r="N24" s="99"/>
+      <c r="O24" s="99"/>
+      <c r="P24" s="99"/>
+      <c r="Q24" s="99"/>
+      <c r="R24" s="100"/>
     </row>
     <row r="25" spans="1:18" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B25" s="90" t="s">
+      <c r="B25" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="91"/>
-      <c r="I25" s="91"/>
-      <c r="J25" s="91"/>
-      <c r="K25" s="91"/>
-      <c r="L25" s="91"/>
-      <c r="M25" s="91"/>
-      <c r="N25" s="91"/>
-      <c r="O25" s="91"/>
-      <c r="P25" s="91"/>
-      <c r="Q25" s="91"/>
-      <c r="R25" s="92"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="90"/>
+      <c r="H25" s="90"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="90"/>
+      <c r="N25" s="90"/>
+      <c r="O25" s="90"/>
+      <c r="P25" s="90"/>
+      <c r="Q25" s="90"/>
+      <c r="R25" s="91"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="R26" s="2"/>
@@ -4757,6 +4778,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="C1AqtvqKb8C414s7lEoNpdJ58hWR+bz87IU733aDeZMTPECU7crf3JYNQw8QcQksZnMw+dDwa8mNa2TsA5r9Aw==" saltValue="4/m+8HEyihP2IsZnh8JafA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="16">
+    <mergeCell ref="B10:R10"/>
+    <mergeCell ref="B14:R14"/>
+    <mergeCell ref="B9:R9"/>
+    <mergeCell ref="B12:R12"/>
+    <mergeCell ref="B7:R7"/>
+    <mergeCell ref="B11:R11"/>
+    <mergeCell ref="B13:R13"/>
     <mergeCell ref="B22:R22"/>
     <mergeCell ref="B23:R23"/>
     <mergeCell ref="B25:R25"/>
@@ -4766,13 +4794,6 @@
     <mergeCell ref="B18:R18"/>
     <mergeCell ref="B19:R19"/>
     <mergeCell ref="B24:R24"/>
-    <mergeCell ref="B10:R10"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B9:R9"/>
-    <mergeCell ref="B12:R12"/>
-    <mergeCell ref="B7:R7"/>
-    <mergeCell ref="B11:R11"/>
-    <mergeCell ref="B13:R13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -10661,8 +10682,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:R202"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H145" sqref="H145"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F153" sqref="F153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10759,7 +10780,7 @@
       </c>
       <c r="J4" s="41">
         <f>I202</f>
-        <v>652.99999999970896</v>
+        <v>701.99999999965075</v>
       </c>
       <c r="L4" s="133"/>
       <c r="R4" t="s">
@@ -10778,7 +10799,7 @@
       </c>
       <c r="J5" s="41">
         <f>J3-J4</f>
-        <v>890.00000000029104</v>
+        <v>841.00000000034925</v>
       </c>
       <c r="L5" s="133"/>
       <c r="M5" s="32"/>
@@ -14654,131 +14675,227 @@
       </c>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B145" s="9"/>
-      <c r="C145" s="9"/>
-      <c r="D145" s="9"/>
-      <c r="E145" s="82" t="str">
+      <c r="B145" s="9" t="s">
+        <v>530</v>
+      </c>
+      <c r="C145" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D145" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="E145" s="82">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F145" s="12"/>
-      <c r="G145" s="12"/>
-      <c r="H145" s="11"/>
-      <c r="I145" s="36" t="str">
+        <v>509.99999999650754</v>
+      </c>
+      <c r="F145" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G145" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="H145" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I145" s="36">
         <f t="shared" si="5"/>
-        <v/>
+        <v>8.4999999999417923</v>
       </c>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B146" s="9"/>
-      <c r="C146" s="9"/>
-      <c r="D146" s="9"/>
-      <c r="E146" s="82" t="str">
+      <c r="B146" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="C146" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D146" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="E146" s="82">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F146" s="12"/>
-      <c r="G146" s="12"/>
-      <c r="H146" s="11"/>
-      <c r="I146" s="36" t="str">
+        <v>210.00000000349246</v>
+      </c>
+      <c r="F146" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G146" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="H146" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I146" s="36">
         <f t="shared" si="5"/>
-        <v/>
+        <v>3.5000000000582077</v>
       </c>
     </row>
     <row r="147" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B147" s="9"/>
-      <c r="C147" s="9"/>
-      <c r="D147" s="9"/>
-      <c r="E147" s="82" t="str">
+      <c r="B147" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="C147" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="D147" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="E147" s="82">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F147" s="12"/>
-      <c r="G147" s="12"/>
-      <c r="H147" s="11"/>
-      <c r="I147" s="36" t="str">
+        <v>270</v>
+      </c>
+      <c r="F147" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G147" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="H147" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I147" s="36">
         <f t="shared" si="5"/>
-        <v/>
+        <v>4.5</v>
       </c>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B148" s="9"/>
-      <c r="C148" s="9"/>
-      <c r="D148" s="9"/>
-      <c r="E148" s="82" t="str">
+      <c r="B148" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="C148" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="D148" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="E148" s="82">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F148" s="12"/>
-      <c r="G148" s="12"/>
-      <c r="H148" s="11"/>
-      <c r="I148" s="36" t="str">
+        <v>180</v>
+      </c>
+      <c r="F148" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G148" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="H148" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I148" s="36">
         <f t="shared" si="5"/>
-        <v/>
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B149" s="9"/>
-      <c r="C149" s="9"/>
-      <c r="D149" s="9"/>
-      <c r="E149" s="82" t="str">
+      <c r="B149" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="C149" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D149" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="E149" s="82">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F149" s="12"/>
-      <c r="G149" s="12"/>
-      <c r="H149" s="11"/>
-      <c r="I149" s="36" t="str">
+        <v>480.00000000349246</v>
+      </c>
+      <c r="F149" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G149" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="H149" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I149" s="36">
         <f t="shared" si="5"/>
-        <v/>
+        <v>8.0000000000582077</v>
       </c>
     </row>
     <row r="150" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B150" s="9"/>
-      <c r="C150" s="9"/>
-      <c r="D150" s="9"/>
-      <c r="E150" s="82" t="str">
+      <c r="B150" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="C150" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D150" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="E150" s="82">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F150" s="12"/>
-      <c r="G150" s="12"/>
-      <c r="H150" s="11"/>
-      <c r="I150" s="36" t="str">
+        <v>360</v>
+      </c>
+      <c r="F150" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G150" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="H150" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I150" s="36">
         <f t="shared" si="5"/>
-        <v/>
+        <v>6</v>
       </c>
     </row>
     <row r="151" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B151" s="9"/>
-      <c r="C151" s="9"/>
-      <c r="D151" s="9"/>
-      <c r="E151" s="82" t="str">
+      <c r="B151" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="C151" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="D151" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="E151" s="82">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F151" s="12"/>
-      <c r="G151" s="12"/>
-      <c r="H151" s="11"/>
-      <c r="I151" s="36" t="str">
+        <v>329.99999999650754</v>
+      </c>
+      <c r="F151" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G151" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="H151" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I151" s="36">
         <f t="shared" si="5"/>
-        <v/>
+        <v>5.4999999999417923</v>
       </c>
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B152" s="9"/>
-      <c r="C152" s="9"/>
-      <c r="D152" s="9"/>
-      <c r="E152" s="82" t="str">
+      <c r="B152" s="9" t="s">
+        <v>536</v>
+      </c>
+      <c r="C152" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D152" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="E152" s="82">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F152" s="12"/>
-      <c r="G152" s="12"/>
-      <c r="H152" s="11"/>
-      <c r="I152" s="36" t="str">
+        <v>599.99999999650754</v>
+      </c>
+      <c r="F152" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G152" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="H152" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I152" s="36">
         <f t="shared" si="5"/>
-        <v/>
+        <v>9.9999999999417923</v>
       </c>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.3">
@@ -15577,7 +15694,7 @@
       <c r="H202" s="35"/>
       <c r="I202" s="83">
         <f>SUM($I$8:I201)</f>
-        <v>652.99999999970896</v>
+        <v>701.99999999965075</v>
       </c>
     </row>
   </sheetData>
@@ -79249,9 +79366,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -79484,19 +79604,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E15B46B-DB71-477E-9F64-462B1A7F47C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5ECEC2-D611-47E4-BF40-446047C7D564}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -79521,9 +79637,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5ECEC2-D611-47E4-BF40-446047C7D564}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E15B46B-DB71-477E-9F64-462B1A7F47C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>